<commit_message>
cambio en hoja de resultados
</commit_message>
<xml_diff>
--- a/Documentos regulatorios.xlsx
+++ b/Documentos regulatorios.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sintec-my.sharepoint.com/personal/zuly_buitrago_sintec_com/Documents/oxxo/Propuesta Comercial/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sintec-my.sharepoint.com/personal/zuly_buitrago_sintec_com/Documents/oxxo/Propuesta Comercial/Lectura_Documentos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="71" documentId="8_{108CE157-D16B-4202-BF58-B068EF40EC5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F22BEFB-D615-4A7F-ACE1-EA96455E9DA1}"/>
+  <xr:revisionPtr revIDLastSave="81" documentId="8_{108CE157-D16B-4202-BF58-B068EF40EC5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B8A1AF8A-47AB-4F6C-897D-14767F05CA77}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{ECA4A055-9DC8-4E48-8F38-B7E6899CCE69}"/>
   </bookViews>
@@ -443,8 +443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67DBD7B6-0996-4F3F-AC60-C2E410CF3C89}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21:C25"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23:B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -499,7 +499,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
@@ -597,7 +597,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C11" t="s">
         <v>14</v>
@@ -611,7 +611,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C12" t="s">
         <v>14</v>
@@ -653,7 +653,7 @@
         <v>10</v>
       </c>
       <c r="B15">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C15" t="s">
         <v>15</v>
@@ -667,7 +667,7 @@
         <v>10</v>
       </c>
       <c r="B16">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C16" t="s">
         <v>15</v>
@@ -681,7 +681,7 @@
         <v>10</v>
       </c>
       <c r="B17">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C17" t="s">
         <v>15</v>
@@ -695,7 +695,7 @@
         <v>11</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C18" t="s">
         <v>16</v>
@@ -709,7 +709,7 @@
         <v>11</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C19" t="s">
         <v>16</v>
@@ -723,7 +723,7 @@
         <v>11</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C20" t="s">
         <v>16</v>
@@ -765,7 +765,7 @@
         <v>11</v>
       </c>
       <c r="B23">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C23" t="s">
         <v>17</v>
@@ -779,7 +779,7 @@
         <v>11</v>
       </c>
       <c r="B24">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C24" t="s">
         <v>17</v>
@@ -793,7 +793,7 @@
         <v>11</v>
       </c>
       <c r="B25">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C25" t="s">
         <v>17</v>

</xml_diff>